<commit_message>
fix bug redmine #114312
</commit_message>
<xml_diff>
--- a/nts.uk/uk.at/at.file/nts.uk.file.at.infra/src/main/resources/report/KWR001_Date_Small_Size.xlsx
+++ b/nts.uk/uk.at/at.file/nts.uk.file.at.infra/src/main/resources/report/KWR001_Date_Small_Size.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23231"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\00_Projects\12_UK\Git\UniversalK\nts.uk\uk.at\at.file\nts.uk.file.at.infra\src\main\resources\report\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nws\Desktop\KWR001_SuaExcel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3543AA8B-A8C3-4BC8-8C29-A31B98167A1F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="3" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="★日別勤務表-個人1行" sheetId="10" r:id="rId1"/>
@@ -116,17 +115,17 @@
     <definedName name="・面接から採用に至るまでの情報管理とする。___・アウトソーシングにて_採用された情報を_ファイ__ルにて取込を行う。" localSheetId="7">#REF!</definedName>
     <definedName name="・面接から採用に至るまでの情報管理とする。___・アウトソーシングにて_採用された情報を_ファイ__ルにて取込を行う。" localSheetId="6">#REF!</definedName>
     <definedName name="・面接から採用に至るまでの情報管理とする。___・アウトソーシングにて_採用された情報を_ファイ__ルにて取込を行う。">#REF!</definedName>
-    <definedName name="a" localSheetId="0">'[1]１．社内ﾈｯﾄﾜｰｸﾊｰﾄﾞｳｪｱ'!#REF!</definedName>
-    <definedName name="a" localSheetId="1">'[1]１．社内ﾈｯﾄﾜｰｸﾊｰﾄﾞｳｪｱ'!#REF!</definedName>
-    <definedName name="a" localSheetId="2">'[1]１．社内ﾈｯﾄﾜｰｸﾊｰﾄﾞｳｪｱ'!#REF!</definedName>
-    <definedName name="a" localSheetId="3">'[1]１．社内ﾈｯﾄﾜｰｸﾊｰﾄﾞｳｪｱ'!#REF!</definedName>
-    <definedName name="a" localSheetId="4">'[1]１．社内ﾈｯﾄﾜｰｸﾊｰﾄﾞｳｪｱ'!#REF!</definedName>
-    <definedName name="a" localSheetId="5">'[1]１．社内ﾈｯﾄﾜｰｸﾊｰﾄﾞｳｪｱ'!#REF!</definedName>
-    <definedName name="a" localSheetId="9">'[1]１．社内ﾈｯﾄﾜｰｸﾊｰﾄﾞｳｪｱ'!#REF!</definedName>
-    <definedName name="a" localSheetId="8">'[1]１．社内ﾈｯﾄﾜｰｸﾊｰﾄﾞｳｪｱ'!#REF!</definedName>
-    <definedName name="a" localSheetId="7">'[1]１．社内ﾈｯﾄﾜｰｸﾊｰﾄﾞｳｪｱ'!#REF!</definedName>
-    <definedName name="a" localSheetId="6">'[1]１．社内ﾈｯﾄﾜｰｸﾊｰﾄﾞｳｪｱ'!#REF!</definedName>
-    <definedName name="a">'[1]１．社内ﾈｯﾄﾜｰｸﾊｰﾄﾞｳｪｱ'!#REF!</definedName>
+    <definedName name="a" localSheetId="0">[1]１．社内ﾈｯﾄﾜｰｸﾊｰﾄﾞｳｪｱ!#REF!</definedName>
+    <definedName name="a" localSheetId="1">[1]１．社内ﾈｯﾄﾜｰｸﾊｰﾄﾞｳｪｱ!#REF!</definedName>
+    <definedName name="a" localSheetId="2">[1]１．社内ﾈｯﾄﾜｰｸﾊｰﾄﾞｳｪｱ!#REF!</definedName>
+    <definedName name="a" localSheetId="3">[1]１．社内ﾈｯﾄﾜｰｸﾊｰﾄﾞｳｪｱ!#REF!</definedName>
+    <definedName name="a" localSheetId="4">[1]１．社内ﾈｯﾄﾜｰｸﾊｰﾄﾞｳｪｱ!#REF!</definedName>
+    <definedName name="a" localSheetId="5">[1]１．社内ﾈｯﾄﾜｰｸﾊｰﾄﾞｳｪｱ!#REF!</definedName>
+    <definedName name="a" localSheetId="9">[1]１．社内ﾈｯﾄﾜｰｸﾊｰﾄﾞｳｪｱ!#REF!</definedName>
+    <definedName name="a" localSheetId="8">[1]１．社内ﾈｯﾄﾜｰｸﾊｰﾄﾞｳｪｱ!#REF!</definedName>
+    <definedName name="a" localSheetId="7">[1]１．社内ﾈｯﾄﾜｰｸﾊｰﾄﾞｳｪｱ!#REF!</definedName>
+    <definedName name="a" localSheetId="6">[1]１．社内ﾈｯﾄﾜｰｸﾊｰﾄﾞｳｪｱ!#REF!</definedName>
+    <definedName name="a">[1]１．社内ﾈｯﾄﾜｰｸﾊｰﾄﾞｳｪｱ!#REF!</definedName>
     <definedName name="AAA" localSheetId="0">#REF!</definedName>
     <definedName name="AAA" localSheetId="1">#REF!</definedName>
     <definedName name="AAA" localSheetId="2">#REF!</definedName>
@@ -368,17 +367,17 @@
     <definedName name="Ｍホ" localSheetId="7">#REF!</definedName>
     <definedName name="Ｍホ" localSheetId="6">#REF!</definedName>
     <definedName name="Ｍホ">#REF!</definedName>
-    <definedName name="ｎ" localSheetId="0">'[4]１．社内ﾈｯﾄﾜｰｸﾊｰﾄﾞｳｪｱ'!#REF!</definedName>
-    <definedName name="ｎ" localSheetId="1">'[4]１．社内ﾈｯﾄﾜｰｸﾊｰﾄﾞｳｪｱ'!#REF!</definedName>
-    <definedName name="ｎ" localSheetId="2">'[4]１．社内ﾈｯﾄﾜｰｸﾊｰﾄﾞｳｪｱ'!#REF!</definedName>
-    <definedName name="ｎ" localSheetId="3">'[4]１．社内ﾈｯﾄﾜｰｸﾊｰﾄﾞｳｪｱ'!#REF!</definedName>
-    <definedName name="ｎ" localSheetId="4">'[4]１．社内ﾈｯﾄﾜｰｸﾊｰﾄﾞｳｪｱ'!#REF!</definedName>
-    <definedName name="ｎ" localSheetId="5">'[4]１．社内ﾈｯﾄﾜｰｸﾊｰﾄﾞｳｪｱ'!#REF!</definedName>
-    <definedName name="ｎ" localSheetId="9">'[4]１．社内ﾈｯﾄﾜｰｸﾊｰﾄﾞｳｪｱ'!#REF!</definedName>
-    <definedName name="ｎ" localSheetId="8">'[4]１．社内ﾈｯﾄﾜｰｸﾊｰﾄﾞｳｪｱ'!#REF!</definedName>
-    <definedName name="ｎ" localSheetId="7">'[4]１．社内ﾈｯﾄﾜｰｸﾊｰﾄﾞｳｪｱ'!#REF!</definedName>
-    <definedName name="ｎ" localSheetId="6">'[4]１．社内ﾈｯﾄﾜｰｸﾊｰﾄﾞｳｪｱ'!#REF!</definedName>
-    <definedName name="ｎ">'[4]１．社内ﾈｯﾄﾜｰｸﾊｰﾄﾞｳｪｱ'!#REF!</definedName>
+    <definedName name="ｎ" localSheetId="0">[4]１．社内ﾈｯﾄﾜｰｸﾊｰﾄﾞｳｪｱ!#REF!</definedName>
+    <definedName name="ｎ" localSheetId="1">[4]１．社内ﾈｯﾄﾜｰｸﾊｰﾄﾞｳｪｱ!#REF!</definedName>
+    <definedName name="ｎ" localSheetId="2">[4]１．社内ﾈｯﾄﾜｰｸﾊｰﾄﾞｳｪｱ!#REF!</definedName>
+    <definedName name="ｎ" localSheetId="3">[4]１．社内ﾈｯﾄﾜｰｸﾊｰﾄﾞｳｪｱ!#REF!</definedName>
+    <definedName name="ｎ" localSheetId="4">[4]１．社内ﾈｯﾄﾜｰｸﾊｰﾄﾞｳｪｱ!#REF!</definedName>
+    <definedName name="ｎ" localSheetId="5">[4]１．社内ﾈｯﾄﾜｰｸﾊｰﾄﾞｳｪｱ!#REF!</definedName>
+    <definedName name="ｎ" localSheetId="9">[4]１．社内ﾈｯﾄﾜｰｸﾊｰﾄﾞｳｪｱ!#REF!</definedName>
+    <definedName name="ｎ" localSheetId="8">[4]１．社内ﾈｯﾄﾜｰｸﾊｰﾄﾞｳｪｱ!#REF!</definedName>
+    <definedName name="ｎ" localSheetId="7">[4]１．社内ﾈｯﾄﾜｰｸﾊｰﾄﾞｳｪｱ!#REF!</definedName>
+    <definedName name="ｎ" localSheetId="6">[4]１．社内ﾈｯﾄﾜｰｸﾊｰﾄﾞｳｪｱ!#REF!</definedName>
+    <definedName name="ｎ">[4]１．社内ﾈｯﾄﾜｰｸﾊｰﾄﾞｳｪｱ!#REF!</definedName>
     <definedName name="ＯＨ" localSheetId="0">#REF!</definedName>
     <definedName name="ＯＨ" localSheetId="1">#REF!</definedName>
     <definedName name="ＯＨ" localSheetId="2">#REF!</definedName>
@@ -678,28 +677,28 @@
     <definedName name="クホ" localSheetId="7">#REF!</definedName>
     <definedName name="クホ" localSheetId="6">#REF!</definedName>
     <definedName name="クホ">#REF!</definedName>
-    <definedName name="サＨ" localSheetId="0">'[8]１．社内ﾈｯﾄﾜｰｸﾊｰﾄﾞｳｪｱ'!#REF!</definedName>
-    <definedName name="サＨ" localSheetId="1">'[8]１．社内ﾈｯﾄﾜｰｸﾊｰﾄﾞｳｪｱ'!#REF!</definedName>
-    <definedName name="サＨ" localSheetId="2">'[8]１．社内ﾈｯﾄﾜｰｸﾊｰﾄﾞｳｪｱ'!#REF!</definedName>
-    <definedName name="サＨ" localSheetId="3">'[8]１．社内ﾈｯﾄﾜｰｸﾊｰﾄﾞｳｪｱ'!#REF!</definedName>
-    <definedName name="サＨ" localSheetId="4">'[8]１．社内ﾈｯﾄﾜｰｸﾊｰﾄﾞｳｪｱ'!#REF!</definedName>
-    <definedName name="サＨ" localSheetId="5">'[8]１．社内ﾈｯﾄﾜｰｸﾊｰﾄﾞｳｪｱ'!#REF!</definedName>
-    <definedName name="サＨ" localSheetId="9">'[8]１．社内ﾈｯﾄﾜｰｸﾊｰﾄﾞｳｪｱ'!#REF!</definedName>
-    <definedName name="サＨ" localSheetId="8">'[8]１．社内ﾈｯﾄﾜｰｸﾊｰﾄﾞｳｪｱ'!#REF!</definedName>
-    <definedName name="サＨ" localSheetId="7">'[8]１．社内ﾈｯﾄﾜｰｸﾊｰﾄﾞｳｪｱ'!#REF!</definedName>
-    <definedName name="サＨ" localSheetId="6">'[8]１．社内ﾈｯﾄﾜｰｸﾊｰﾄﾞｳｪｱ'!#REF!</definedName>
-    <definedName name="サＨ">'[8]１．社内ﾈｯﾄﾜｰｸﾊｰﾄﾞｳｪｱ'!#REF!</definedName>
-    <definedName name="サホ" localSheetId="0">'[8]１．社内ﾈｯﾄﾜｰｸﾊｰﾄﾞｳｪｱ'!#REF!</definedName>
-    <definedName name="サホ" localSheetId="1">'[8]１．社内ﾈｯﾄﾜｰｸﾊｰﾄﾞｳｪｱ'!#REF!</definedName>
-    <definedName name="サホ" localSheetId="2">'[8]１．社内ﾈｯﾄﾜｰｸﾊｰﾄﾞｳｪｱ'!#REF!</definedName>
-    <definedName name="サホ" localSheetId="3">'[8]１．社内ﾈｯﾄﾜｰｸﾊｰﾄﾞｳｪｱ'!#REF!</definedName>
-    <definedName name="サホ" localSheetId="4">'[8]１．社内ﾈｯﾄﾜｰｸﾊｰﾄﾞｳｪｱ'!#REF!</definedName>
-    <definedName name="サホ" localSheetId="5">'[8]１．社内ﾈｯﾄﾜｰｸﾊｰﾄﾞｳｪｱ'!#REF!</definedName>
-    <definedName name="サホ" localSheetId="9">'[8]１．社内ﾈｯﾄﾜｰｸﾊｰﾄﾞｳｪｱ'!#REF!</definedName>
-    <definedName name="サホ" localSheetId="8">'[8]１．社内ﾈｯﾄﾜｰｸﾊｰﾄﾞｳｪｱ'!#REF!</definedName>
-    <definedName name="サホ" localSheetId="7">'[8]１．社内ﾈｯﾄﾜｰｸﾊｰﾄﾞｳｪｱ'!#REF!</definedName>
-    <definedName name="サホ" localSheetId="6">'[8]１．社内ﾈｯﾄﾜｰｸﾊｰﾄﾞｳｪｱ'!#REF!</definedName>
-    <definedName name="サホ">'[8]１．社内ﾈｯﾄﾜｰｸﾊｰﾄﾞｳｪｱ'!#REF!</definedName>
+    <definedName name="サＨ" localSheetId="0">[8]１．社内ﾈｯﾄﾜｰｸﾊｰﾄﾞｳｪｱ!#REF!</definedName>
+    <definedName name="サＨ" localSheetId="1">[8]１．社内ﾈｯﾄﾜｰｸﾊｰﾄﾞｳｪｱ!#REF!</definedName>
+    <definedName name="サＨ" localSheetId="2">[8]１．社内ﾈｯﾄﾜｰｸﾊｰﾄﾞｳｪｱ!#REF!</definedName>
+    <definedName name="サＨ" localSheetId="3">[8]１．社内ﾈｯﾄﾜｰｸﾊｰﾄﾞｳｪｱ!#REF!</definedName>
+    <definedName name="サＨ" localSheetId="4">[8]１．社内ﾈｯﾄﾜｰｸﾊｰﾄﾞｳｪｱ!#REF!</definedName>
+    <definedName name="サＨ" localSheetId="5">[8]１．社内ﾈｯﾄﾜｰｸﾊｰﾄﾞｳｪｱ!#REF!</definedName>
+    <definedName name="サＨ" localSheetId="9">[8]１．社内ﾈｯﾄﾜｰｸﾊｰﾄﾞｳｪｱ!#REF!</definedName>
+    <definedName name="サＨ" localSheetId="8">[8]１．社内ﾈｯﾄﾜｰｸﾊｰﾄﾞｳｪｱ!#REF!</definedName>
+    <definedName name="サＨ" localSheetId="7">[8]１．社内ﾈｯﾄﾜｰｸﾊｰﾄﾞｳｪｱ!#REF!</definedName>
+    <definedName name="サＨ" localSheetId="6">[8]１．社内ﾈｯﾄﾜｰｸﾊｰﾄﾞｳｪｱ!#REF!</definedName>
+    <definedName name="サＨ">[8]１．社内ﾈｯﾄﾜｰｸﾊｰﾄﾞｳｪｱ!#REF!</definedName>
+    <definedName name="サホ" localSheetId="0">[8]１．社内ﾈｯﾄﾜｰｸﾊｰﾄﾞｳｪｱ!#REF!</definedName>
+    <definedName name="サホ" localSheetId="1">[8]１．社内ﾈｯﾄﾜｰｸﾊｰﾄﾞｳｪｱ!#REF!</definedName>
+    <definedName name="サホ" localSheetId="2">[8]１．社内ﾈｯﾄﾜｰｸﾊｰﾄﾞｳｪｱ!#REF!</definedName>
+    <definedName name="サホ" localSheetId="3">[8]１．社内ﾈｯﾄﾜｰｸﾊｰﾄﾞｳｪｱ!#REF!</definedName>
+    <definedName name="サホ" localSheetId="4">[8]１．社内ﾈｯﾄﾜｰｸﾊｰﾄﾞｳｪｱ!#REF!</definedName>
+    <definedName name="サホ" localSheetId="5">[8]１．社内ﾈｯﾄﾜｰｸﾊｰﾄﾞｳｪｱ!#REF!</definedName>
+    <definedName name="サホ" localSheetId="9">[8]１．社内ﾈｯﾄﾜｰｸﾊｰﾄﾞｳｪｱ!#REF!</definedName>
+    <definedName name="サホ" localSheetId="8">[8]１．社内ﾈｯﾄﾜｰｸﾊｰﾄﾞｳｪｱ!#REF!</definedName>
+    <definedName name="サホ" localSheetId="7">[8]１．社内ﾈｯﾄﾜｰｸﾊｰﾄﾞｳｪｱ!#REF!</definedName>
+    <definedName name="サホ" localSheetId="6">[8]１．社内ﾈｯﾄﾜｰｸﾊｰﾄﾞｳｪｱ!#REF!</definedName>
+    <definedName name="サホ">[8]１．社内ﾈｯﾄﾜｰｸﾊｰﾄﾞｳｪｱ!#REF!</definedName>
     <definedName name="サホ1" localSheetId="0">#REF!</definedName>
     <definedName name="サホ1" localSheetId="1">#REF!</definedName>
     <definedName name="サホ1" localSheetId="2">#REF!</definedName>
@@ -1194,7 +1193,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="6">
     <font>
       <sz val="9"/>
@@ -2898,7 +2897,7 @@
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="標準 10" xfId="1" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
+    <cellStyle name="標準 10" xfId="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -46471,7 +46470,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet1">
     <tabColor theme="0" tint="-0.14999847407452621"/>
   </sheetPr>
@@ -46728,11 +46727,11 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet10"/>
   <dimension ref="A1:AX77"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" showWhiteSpace="0" zoomScale="118" zoomScaleNormal="130" zoomScaleSheetLayoutView="110" zoomScalePageLayoutView="118" workbookViewId="0">
+    <sheetView showGridLines="0" showWhiteSpace="0" topLeftCell="A40" zoomScale="118" zoomScaleNormal="130" zoomScaleSheetLayoutView="110" zoomScalePageLayoutView="118" workbookViewId="0">
       <selection activeCell="X14" sqref="X14:Y14"/>
     </sheetView>
   </sheetViews>
@@ -52065,14 +52064,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet2">
     <tabColor theme="0" tint="-0.14999847407452621"/>
   </sheetPr>
   <dimension ref="A1:AU6"/>
   <sheetViews>
     <sheetView showGridLines="0" view="pageLayout" zoomScale="130" zoomScaleNormal="130" zoomScaleSheetLayoutView="85" zoomScalePageLayoutView="130" workbookViewId="0">
-      <selection activeCell="BA13" sqref="BA13"/>
+      <selection activeCell="K22" sqref="K22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="3.140625" defaultRowHeight="15" customHeight="1"/>
@@ -52440,7 +52439,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet3"/>
   <dimension ref="A1:AU8"/>
   <sheetViews>
@@ -52929,11 +52928,11 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet4"/>
   <dimension ref="A1:AU4"/>
   <sheetViews>
-    <sheetView showGridLines="0" view="pageLayout" zoomScale="130" zoomScaleNormal="130" zoomScaleSheetLayoutView="110" zoomScalePageLayoutView="130" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" view="pageLayout" zoomScale="130" zoomScaleNormal="130" zoomScaleSheetLayoutView="110" zoomScalePageLayoutView="130" workbookViewId="0">
       <selection activeCell="AZ9" sqref="AZ9"/>
     </sheetView>
   </sheetViews>
@@ -53177,7 +53176,7 @@
   <pageMargins left="0.39370078740157499" right="0.39370078740157499" top="0.98425196850393704" bottom="0.1" header="0.39370078740157499" footer="0.1"/>
   <pageSetup paperSize="9" orientation="landscape" r:id="rId1"/>
   <headerFooter>
-    <oddHeader>&amp;C&amp;"ＭＳ ゴシック,標準 Bold"&amp;16日別勤務表&amp;R&amp;"ＭＳ ゴシック,標準"&amp;D　&amp;T　
+    <oddHeader>&amp;C&amp;"ＭＳ ゴシック,Regular"&amp;16日別勤務表&amp;R&amp;"ＭＳ ゴシック,Regular"&amp;D　&amp;T　
 page&amp;P</oddHeader>
     <oddFooter xml:space="preserve">&amp;L備考　未マ：マスタ未登録、漏れ：打刻漏れ、打順：打刻順序不正、遅：遅刻、早：早退、休打：休日打刻、二重：二重打刻、反映：承認反映、手：手入力、未計：未計算、申超：事前申請超過 </oddFooter>
   </headerFooter>
@@ -53185,7 +53184,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet5"/>
   <dimension ref="A1:AU6"/>
   <sheetViews>
@@ -53558,7 +53557,7 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet6"/>
   <dimension ref="A1:AU8"/>
   <sheetViews>
@@ -54042,19 +54041,19 @@
   <pageMargins left="0.39370078740157499" right="0.39370078740157499" top="0.98425196850393704" bottom="0.1" header="0.39370078740157499" footer="0.1"/>
   <pageSetup paperSize="9" orientation="landscape" r:id="rId1"/>
   <headerFooter>
-    <oddHeader>&amp;C&amp;"ＭＳ ゴシック,標準 Bold"&amp;16日別勤務表</oddHeader>
+    <oddHeader>&amp;C&amp;"ＭＳ ゴシック,Regular"&amp;16日別勤務表</oddHeader>
     <oddFooter xml:space="preserve">&amp;L備考　未マ：マスタ未登録、漏れ：打刻漏れ、打順：打刻順序不正、遅：遅刻、早：早退、休打：休日打刻、二重：二重打刻、反映：承認反映、手：手入力、未計：未計算、申超：事前申請超過 </oddFooter>
   </headerFooter>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet7"/>
   <dimension ref="A1:AU37"/>
   <sheetViews>
-    <sheetView showGridLines="0" view="pageLayout" topLeftCell="A31" zoomScale="130" zoomScaleNormal="130" zoomScaleSheetLayoutView="85" zoomScalePageLayoutView="130" workbookViewId="0">
-      <selection activeCell="AP3" sqref="AP3:AQ4"/>
+    <sheetView showGridLines="0" view="pageLayout" topLeftCell="A46" zoomScale="130" zoomScaleNormal="130" zoomScaleSheetLayoutView="85" zoomScalePageLayoutView="130" workbookViewId="0">
+      <selection activeCell="AB7" sqref="AB7:AC8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="3.140625" defaultRowHeight="15" customHeight="1"/>
@@ -55579,7 +55578,6 @@
     <mergeCell ref="F21:G21"/>
     <mergeCell ref="H21:I21"/>
     <mergeCell ref="L21:M21"/>
-    <mergeCell ref="J7:K8"/>
     <mergeCell ref="H13:I13"/>
     <mergeCell ref="L13:M13"/>
     <mergeCell ref="F14:G14"/>
@@ -55591,8 +55589,14 @@
     <mergeCell ref="J12:K12"/>
     <mergeCell ref="J13:K13"/>
     <mergeCell ref="J14:K14"/>
-    <mergeCell ref="A10:AU10"/>
-    <mergeCell ref="AR3:AU8"/>
+    <mergeCell ref="N7:O8"/>
+    <mergeCell ref="P7:Q8"/>
+    <mergeCell ref="R7:S8"/>
+    <mergeCell ref="T7:U8"/>
+    <mergeCell ref="V7:W8"/>
+    <mergeCell ref="X7:Y8"/>
+    <mergeCell ref="Z7:AA8"/>
+    <mergeCell ref="AB7:AC8"/>
     <mergeCell ref="A1:W1"/>
     <mergeCell ref="A3:A8"/>
     <mergeCell ref="B3:C8"/>
@@ -55603,28 +55607,11 @@
     <mergeCell ref="T3:U4"/>
     <mergeCell ref="V3:W4"/>
     <mergeCell ref="D5:E6"/>
-    <mergeCell ref="AD7:AE8"/>
-    <mergeCell ref="AF7:AG8"/>
-    <mergeCell ref="AH7:AI8"/>
-    <mergeCell ref="AJ7:AK8"/>
-    <mergeCell ref="AL7:AM8"/>
-    <mergeCell ref="AN7:AO8"/>
-    <mergeCell ref="AP7:AQ8"/>
     <mergeCell ref="D7:E8"/>
     <mergeCell ref="F3:G4"/>
-    <mergeCell ref="D11:E11"/>
+    <mergeCell ref="J7:K8"/>
     <mergeCell ref="X3:Y4"/>
     <mergeCell ref="Z3:AA4"/>
-    <mergeCell ref="AB3:AC4"/>
-    <mergeCell ref="AD3:AE4"/>
-    <mergeCell ref="N7:O8"/>
-    <mergeCell ref="P7:Q8"/>
-    <mergeCell ref="R7:S8"/>
-    <mergeCell ref="T7:U8"/>
-    <mergeCell ref="V7:W8"/>
-    <mergeCell ref="X7:Y8"/>
-    <mergeCell ref="Z7:AA8"/>
-    <mergeCell ref="AB7:AC8"/>
     <mergeCell ref="J11:K11"/>
     <mergeCell ref="H3:I4"/>
     <mergeCell ref="L3:M4"/>
@@ -55636,6 +55623,16 @@
     <mergeCell ref="L7:M8"/>
     <mergeCell ref="J3:K4"/>
     <mergeCell ref="J5:K6"/>
+    <mergeCell ref="A10:AU10"/>
+    <mergeCell ref="AR3:AU8"/>
+    <mergeCell ref="AD7:AE8"/>
+    <mergeCell ref="AF7:AG8"/>
+    <mergeCell ref="AH7:AI8"/>
+    <mergeCell ref="AJ7:AK8"/>
+    <mergeCell ref="AL7:AM8"/>
+    <mergeCell ref="AN7:AO8"/>
+    <mergeCell ref="AP7:AQ8"/>
+    <mergeCell ref="D11:E11"/>
     <mergeCell ref="AJ13:AK13"/>
     <mergeCell ref="A9:AU9"/>
     <mergeCell ref="AP11:AQ11"/>
@@ -56040,13 +56037,14 @@
     <mergeCell ref="AH3:AI4"/>
     <mergeCell ref="AJ3:AK4"/>
     <mergeCell ref="AF3:AG4"/>
+    <mergeCell ref="AB3:AC4"/>
+    <mergeCell ref="AD3:AE4"/>
   </mergeCells>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.39370078740157483" right="0.39370078740157483" top="0.98425196850393704" bottom="0.39370078740157483" header="0.39370078740157483" footer="0.31496062992125984"/>
   <pageSetup paperSize="9" orientation="landscape" r:id="rId1"/>
   <headerFooter>
-    <oddHeader>&amp;C
-&amp;"源ノ角ゴシック Normal,Regular"&amp;16日別勤務表&amp;R&amp;"源ノ角ゴシック Normal,Regular"&amp;D　&amp;T　
+    <oddHeader>&amp;C&amp;"源ノ角ゴシック Normal,Regular"&amp;16日別勤務表&amp;R&amp;"源ノ角ゴシック Normal,Regular"&amp;D　&amp;T　
 page&amp;P</oddHeader>
     <oddFooter xml:space="preserve">&amp;L備考　未マ：マスタ未登録、漏れ：打刻漏れ、打順：打刻順序不正、遅：遅刻、早：早退、休打：休日打刻、二重：二重打刻、反映：承認反映、手：手入力、未計：未計算、申超：事前申請超過 </oddFooter>
   </headerFooter>
@@ -56054,14 +56052,14 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet8">
     <tabColor theme="0" tint="-0.499984740745262"/>
   </sheetPr>
   <dimension ref="A1:AU74"/>
   <sheetViews>
-    <sheetView showGridLines="0" view="pageLayout" topLeftCell="A31" zoomScale="130" zoomScaleNormal="130" zoomScaleSheetLayoutView="85" zoomScalePageLayoutView="130" workbookViewId="0">
-      <selection activeCell="A35" sqref="A35:AU35"/>
+    <sheetView showGridLines="0" view="pageLayout" zoomScale="130" zoomScaleNormal="130" zoomScaleSheetLayoutView="85" zoomScalePageLayoutView="130" workbookViewId="0">
+      <selection activeCell="Z32" sqref="Z32:AA32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="3.140625" defaultRowHeight="15" customHeight="1"/>
@@ -59369,9 +59367,6 @@
     <row r="74" spans="1:47" ht="9.9499999999999993" customHeight="1"/>
   </sheetData>
   <mergeCells count="1224">
-    <mergeCell ref="H66:I66"/>
-    <mergeCell ref="J66:K66"/>
-    <mergeCell ref="L66:M66"/>
     <mergeCell ref="F67:G67"/>
     <mergeCell ref="H67:I67"/>
     <mergeCell ref="J67:K67"/>
@@ -59396,7 +59391,6 @@
     <mergeCell ref="H61:I61"/>
     <mergeCell ref="J61:K61"/>
     <mergeCell ref="L61:M61"/>
-    <mergeCell ref="L52:M52"/>
     <mergeCell ref="F53:G53"/>
     <mergeCell ref="H53:I53"/>
     <mergeCell ref="J53:K53"/>
@@ -59413,10 +59407,9 @@
     <mergeCell ref="H56:I56"/>
     <mergeCell ref="J56:K56"/>
     <mergeCell ref="L56:M56"/>
-    <mergeCell ref="F45:G45"/>
-    <mergeCell ref="H45:I45"/>
-    <mergeCell ref="J45:K45"/>
-    <mergeCell ref="L45:M45"/>
+    <mergeCell ref="H66:I66"/>
+    <mergeCell ref="J66:K66"/>
+    <mergeCell ref="L66:M66"/>
     <mergeCell ref="F46:G46"/>
     <mergeCell ref="H46:I46"/>
     <mergeCell ref="J46:K46"/>
@@ -59433,10 +59426,7 @@
     <mergeCell ref="H49:I49"/>
     <mergeCell ref="J49:K49"/>
     <mergeCell ref="L49:M49"/>
-    <mergeCell ref="F40:G40"/>
-    <mergeCell ref="H40:I40"/>
-    <mergeCell ref="J40:K40"/>
-    <mergeCell ref="L40:M40"/>
+    <mergeCell ref="L52:M52"/>
     <mergeCell ref="F41:G41"/>
     <mergeCell ref="H41:I41"/>
     <mergeCell ref="J41:K41"/>
@@ -59453,12 +59443,10 @@
     <mergeCell ref="H44:I44"/>
     <mergeCell ref="J44:K44"/>
     <mergeCell ref="L44:M44"/>
-    <mergeCell ref="L29:M29"/>
-    <mergeCell ref="F30:G30"/>
-    <mergeCell ref="H30:I30"/>
-    <mergeCell ref="J30:K30"/>
-    <mergeCell ref="L30:M30"/>
-    <mergeCell ref="F31:G31"/>
+    <mergeCell ref="F45:G45"/>
+    <mergeCell ref="H45:I45"/>
+    <mergeCell ref="J45:K45"/>
+    <mergeCell ref="L45:M45"/>
     <mergeCell ref="H31:I31"/>
     <mergeCell ref="J31:K31"/>
     <mergeCell ref="L31:M31"/>
@@ -59472,6 +59460,19 @@
     <mergeCell ref="L36:M36"/>
     <mergeCell ref="A34:AU34"/>
     <mergeCell ref="A35:AU35"/>
+    <mergeCell ref="AR31:AU31"/>
+    <mergeCell ref="AL29:AM29"/>
+    <mergeCell ref="AN29:AO29"/>
+    <mergeCell ref="P30:Q30"/>
+    <mergeCell ref="R30:S30"/>
+    <mergeCell ref="T30:U30"/>
+    <mergeCell ref="V30:W30"/>
+    <mergeCell ref="X30:Y30"/>
+    <mergeCell ref="AJ31:AK31"/>
+    <mergeCell ref="AL31:AM31"/>
+    <mergeCell ref="AF32:AG32"/>
+    <mergeCell ref="AH32:AI32"/>
+    <mergeCell ref="AJ32:AK32"/>
     <mergeCell ref="F23:G23"/>
     <mergeCell ref="H23:I23"/>
     <mergeCell ref="J23:K23"/>
@@ -59886,9 +59887,6 @@
     <mergeCell ref="AF29:AG29"/>
     <mergeCell ref="AH29:AI29"/>
     <mergeCell ref="AJ29:AK29"/>
-    <mergeCell ref="AR31:AU31"/>
-    <mergeCell ref="AL29:AM29"/>
-    <mergeCell ref="AN29:AO29"/>
     <mergeCell ref="AR28:AU28"/>
     <mergeCell ref="D29:E29"/>
     <mergeCell ref="N29:O29"/>
@@ -59918,16 +59916,7 @@
     <mergeCell ref="F29:G29"/>
     <mergeCell ref="H29:I29"/>
     <mergeCell ref="J29:K29"/>
-    <mergeCell ref="P30:Q30"/>
-    <mergeCell ref="R30:S30"/>
-    <mergeCell ref="T30:U30"/>
-    <mergeCell ref="V30:W30"/>
-    <mergeCell ref="X30:Y30"/>
-    <mergeCell ref="AJ31:AK31"/>
-    <mergeCell ref="AL31:AM31"/>
-    <mergeCell ref="AF32:AG32"/>
-    <mergeCell ref="AH32:AI32"/>
-    <mergeCell ref="AJ32:AK32"/>
+    <mergeCell ref="L29:M29"/>
     <mergeCell ref="AL32:AM32"/>
     <mergeCell ref="AN32:AO32"/>
     <mergeCell ref="AP32:AQ32"/>
@@ -59955,6 +59944,11 @@
     <mergeCell ref="AL30:AM30"/>
     <mergeCell ref="AN30:AO30"/>
     <mergeCell ref="AP30:AQ30"/>
+    <mergeCell ref="F30:G30"/>
+    <mergeCell ref="H30:I30"/>
+    <mergeCell ref="J30:K30"/>
+    <mergeCell ref="L30:M30"/>
+    <mergeCell ref="F31:G31"/>
     <mergeCell ref="AR30:AU30"/>
     <mergeCell ref="D31:E31"/>
     <mergeCell ref="N31:O31"/>
@@ -59972,12 +59966,21 @@
     <mergeCell ref="D30:E30"/>
     <mergeCell ref="N30:O30"/>
     <mergeCell ref="AR38:AU38"/>
-    <mergeCell ref="D39:E39"/>
-    <mergeCell ref="N39:O39"/>
-    <mergeCell ref="R36:S36"/>
-    <mergeCell ref="T36:U36"/>
-    <mergeCell ref="V36:W36"/>
-    <mergeCell ref="X36:Y36"/>
+    <mergeCell ref="AD37:AE37"/>
+    <mergeCell ref="AF37:AG37"/>
+    <mergeCell ref="AH37:AI37"/>
+    <mergeCell ref="AJ37:AK37"/>
+    <mergeCell ref="AL37:AM37"/>
+    <mergeCell ref="AP36:AQ36"/>
+    <mergeCell ref="AR36:AU36"/>
+    <mergeCell ref="D37:E37"/>
+    <mergeCell ref="N37:O37"/>
+    <mergeCell ref="P37:Q37"/>
+    <mergeCell ref="R37:S37"/>
+    <mergeCell ref="T37:U37"/>
+    <mergeCell ref="V37:W37"/>
+    <mergeCell ref="X37:Y37"/>
+    <mergeCell ref="Z37:AA37"/>
     <mergeCell ref="Z36:AA36"/>
     <mergeCell ref="AB36:AC36"/>
     <mergeCell ref="A36:A37"/>
@@ -60004,21 +60007,6 @@
     <mergeCell ref="Z33:AA33"/>
     <mergeCell ref="AB33:AC33"/>
     <mergeCell ref="AB37:AC37"/>
-    <mergeCell ref="AD37:AE37"/>
-    <mergeCell ref="AF37:AG37"/>
-    <mergeCell ref="AH37:AI37"/>
-    <mergeCell ref="AJ37:AK37"/>
-    <mergeCell ref="AL37:AM37"/>
-    <mergeCell ref="AP36:AQ36"/>
-    <mergeCell ref="AR36:AU36"/>
-    <mergeCell ref="D37:E37"/>
-    <mergeCell ref="N37:O37"/>
-    <mergeCell ref="P37:Q37"/>
-    <mergeCell ref="R37:S37"/>
-    <mergeCell ref="T37:U37"/>
-    <mergeCell ref="V37:W37"/>
-    <mergeCell ref="X37:Y37"/>
-    <mergeCell ref="Z37:AA37"/>
     <mergeCell ref="AD36:AE36"/>
     <mergeCell ref="AF36:AG36"/>
     <mergeCell ref="AH36:AI36"/>
@@ -60046,6 +60034,11 @@
     <mergeCell ref="Z38:AA38"/>
     <mergeCell ref="AB38:AC38"/>
     <mergeCell ref="AD38:AE38"/>
+    <mergeCell ref="N39:O39"/>
+    <mergeCell ref="R36:S36"/>
+    <mergeCell ref="T36:U36"/>
+    <mergeCell ref="V36:W36"/>
+    <mergeCell ref="X36:Y36"/>
     <mergeCell ref="A38:A39"/>
     <mergeCell ref="B38:B39"/>
     <mergeCell ref="C38:C39"/>
@@ -60063,6 +60056,11 @@
     <mergeCell ref="L39:M39"/>
     <mergeCell ref="AH40:AI40"/>
     <mergeCell ref="AJ40:AK40"/>
+    <mergeCell ref="D39:E39"/>
+    <mergeCell ref="F40:G40"/>
+    <mergeCell ref="H40:I40"/>
+    <mergeCell ref="J40:K40"/>
+    <mergeCell ref="L40:M40"/>
     <mergeCell ref="AL40:AM40"/>
     <mergeCell ref="AN40:AO40"/>
     <mergeCell ref="AP40:AQ40"/>
@@ -60598,8 +60596,7 @@
   <pageMargins left="0.39370078740157499" right="0.39370078740157499" top="0.98425196850393704" bottom="0.1" header="0.39370078740157499" footer="0.1"/>
   <pageSetup paperSize="9" orientation="landscape" r:id="rId1"/>
   <headerFooter>
-    <oddHeader>&amp;C
-&amp;"源ノ角ゴシック Normal,Regular"&amp;16日別勤務表&amp;R&amp;"源ノ角ゴシック Normal,Regular"&amp;D　&amp;T　
+    <oddHeader>&amp;C&amp;"源ノ角ゴシック Normal,Regular"&amp;16日別勤務表&amp;R&amp;"源ノ角ゴシック Normal,Regular"&amp;D　&amp;T　
 page&amp;P</oddHeader>
     <oddFooter xml:space="preserve">&amp;L備考　未マ：マスタ未登録、漏れ：打刻漏れ、打順：打刻順序不正、遅：遅刻、早：早退、休打：休日打刻、二重：二重打刻、反映：承認反映、手：手入力、未計：未計算、申超：事前申請超過 </oddFooter>
   </headerFooter>
@@ -60607,14 +60604,14 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet9">
     <tabColor theme="0" tint="-0.499984740745262"/>
   </sheetPr>
   <dimension ref="A1:AU44"/>
   <sheetViews>
     <sheetView showGridLines="0" view="pageLayout" zoomScale="130" zoomScaleNormal="130" zoomScaleSheetLayoutView="85" zoomScalePageLayoutView="130" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7:AU7"/>
+      <selection activeCell="AB4" sqref="AB4:AC5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="3.140625" defaultRowHeight="15" customHeight="1"/>

</xml_diff>